<commit_message>
Automatizzazione del file ottimizzazione
</commit_message>
<xml_diff>
--- a/Shading Trees/Shock/Shading_trees.xlsx
+++ b/Shading Trees/Shock/Shading_trees.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\payam\Documents\GitHub\CIVICS_Kenya\Shading Trees\Shock\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gollinucci\Documents\GitHub\CIVICS_Kenya\Shading Trees\Shock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086DC514-4272-4341-97BE-FCDF328FC9BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEB4AF5-D382-4FE2-B60C-103967E671D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S" sheetId="7" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="268">
   <si>
     <t>level_row</t>
   </si>
@@ -857,6 +857,9 @@
   </si>
   <si>
     <t>Residential</t>
+  </si>
+  <si>
+    <t>numbeo</t>
   </si>
 </sst>
 </file>
@@ -864,8 +867,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0;\-;\-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0;\-;\-"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -1032,7 +1035,7 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -1085,7 +1088,7 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1736,7 +1739,7 @@
       </c>
       <c r="G3" s="54">
         <f>main!C34</f>
-        <v>-6.5496463190985022E-5</v>
+        <v>-9.6685255186692185E-5</v>
       </c>
       <c r="H3" s="54" t="s">
         <v>204</v>
@@ -2633,10 +2636,10 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D38" sqref="D38"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2825,7 +2828,7 @@
         <v>241</v>
       </c>
       <c r="C8" s="19">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>244</v>
@@ -2857,7 +2860,8 @@
         <v>240</v>
       </c>
       <c r="C9" s="19">
-        <v>7</v>
+        <f>162-7</f>
+        <v>155</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>245</v>
@@ -2869,7 +2873,7 @@
       <c r="I9" s="48"/>
       <c r="J9" s="10"/>
       <c r="K9" s="24" t="s">
-        <v>246</v>
+        <v>267</v>
       </c>
       <c r="L9" s="23"/>
     </row>
@@ -3149,7 +3153,7 @@
       </c>
       <c r="C24" s="14">
         <f>C9*C8*C6*C5*C3/1000000</f>
-        <v>4634.5950000000003</v>
+        <v>6841.5450000000001</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>190</v>
@@ -3360,7 +3364,7 @@
       </c>
       <c r="C34" s="32">
         <f>-C24*C18/C10</f>
-        <v>-6.5496463190985022E-5</v>
+        <v>-9.6685255186692185E-5</v>
       </c>
       <c r="D34" s="28"/>
       <c r="E34" s="47"/>
@@ -3410,9 +3414,10 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K7" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="K9" r:id="rId2" xr:uid="{AD77FBCA-DB57-49E0-B1C8-34C2897E5A3B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actual version of Shading_trees shock values
</commit_message>
<xml_diff>
--- a/Shading Trees/Shock/Shading_trees.xlsx
+++ b/Shading Trees/Shock/Shading_trees.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gollinucci\Documents\GitHub\CIVICS_Kenya\Shading Trees\Shock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEB4AF5-D382-4FE2-B60C-103967E671D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06487B3-E949-4549-882B-B396D39BBAEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S" sheetId="7" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="267">
   <si>
     <t>level_row</t>
   </si>
@@ -857,9 +857,6 @@
   </si>
   <si>
     <t>Residential</t>
-  </si>
-  <si>
-    <t>numbeo</t>
   </si>
 </sst>
 </file>
@@ -1739,7 +1736,7 @@
       </c>
       <c r="G3" s="54">
         <f>main!C34</f>
-        <v>-9.6685255186692185E-5</v>
+        <v>-6.5496463190985022E-5</v>
       </c>
       <c r="H3" s="54" t="s">
         <v>204</v>
@@ -2639,7 +2636,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2828,7 +2825,7 @@
         <v>241</v>
       </c>
       <c r="C8" s="19">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>244</v>
@@ -2860,8 +2857,7 @@
         <v>240</v>
       </c>
       <c r="C9" s="19">
-        <f>162-7</f>
-        <v>155</v>
+        <v>7</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>245</v>
@@ -2873,7 +2869,7 @@
       <c r="I9" s="48"/>
       <c r="J9" s="10"/>
       <c r="K9" s="24" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="L9" s="23"/>
     </row>
@@ -3153,7 +3149,7 @@
       </c>
       <c r="C24" s="14">
         <f>C9*C8*C6*C5*C3/1000000</f>
-        <v>6841.5450000000001</v>
+        <v>4634.5950000000003</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>190</v>
@@ -3364,7 +3360,7 @@
       </c>
       <c r="C34" s="32">
         <f>-C24*C18/C10</f>
-        <v>-9.6685255186692185E-5</v>
+        <v>-6.5496463190985022E-5</v>
       </c>
       <c r="D34" s="28"/>
       <c r="E34" s="47"/>
@@ -3414,10 +3410,9 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K7" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="K9" r:id="rId2" xr:uid="{AD77FBCA-DB57-49E0-B1C8-34C2897E5A3B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>